<commit_message>
Show more/fewer fields in a Fast Tab
</commit_message>
<xml_diff>
--- a/TC_CreateEmployees/Main.rvl.xlsx
+++ b/TC_CreateEmployees/Main.rvl.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="181">
   <si>
     <t>Flow</t>
   </si>
@@ -528,6 +528,36 @@
   </si>
   <si>
     <t>100</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>showMoreFields</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>toggleAdditionalFields</t>
+  </si>
+  <si>
+    <t>additionalFieldsButtonName</t>
+  </si>
+  <si>
+    <t>Show less fields</t>
+  </si>
+  <si>
+    <t>Show fewer fields</t>
+  </si>
+  <si>
+    <t>Invoice Details</t>
+  </si>
+  <si>
+    <t>Show more fields</t>
   </si>
 </sst>
 </file>
@@ -4479,7 +4509,7 @@
         <v>14</v>
       </c>
       <c r="G4" s="658" t="s">
-        <v>167</v>
+        <v>24</v>
       </c>
       <c r="H4" s="659"/>
     </row>
@@ -4510,32 +4540,60 @@
     </row>
     <row r="7">
       <c r="A7" s="668"/>
-      <c r="B7" s="669"/>
-      <c r="C7" s="670"/>
-      <c r="D7" s="671"/>
-      <c r="E7" s="672"/>
-      <c r="F7" s="673"/>
-      <c r="G7" s="674"/>
+      <c r="B7" s="669" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="670" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="671" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="672" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="673" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="674" t="s">
+        <v>179</v>
+      </c>
       <c r="H7" s="675"/>
     </row>
     <row r="8">
       <c r="A8" s="676"/>
-      <c r="B8" s="677"/>
+      <c r="B8" s="677" t="s">
+        <v>18</v>
+      </c>
       <c r="C8" s="678"/>
       <c r="D8" s="679"/>
-      <c r="E8" s="680"/>
-      <c r="F8" s="681"/>
-      <c r="G8" s="682"/>
+      <c r="E8" s="680" t="s">
+        <v>175</v>
+      </c>
+      <c r="F8" s="681" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="682" t="s">
+        <v>173</v>
+      </c>
       <c r="H8" s="683"/>
     </row>
     <row r="9">
       <c r="A9" s="684"/>
-      <c r="B9" s="685"/>
+      <c r="B9" s="685" t="s">
+        <v>18</v>
+      </c>
       <c r="C9" s="686"/>
       <c r="D9" s="687"/>
-      <c r="E9" s="688"/>
-      <c r="F9" s="689"/>
-      <c r="G9" s="690"/>
+      <c r="E9" s="688" t="s">
+        <v>176</v>
+      </c>
+      <c r="F9" s="689" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="690" t="s">
+        <v>180</v>
+      </c>
       <c r="H9" s="691"/>
     </row>
     <row r="10">

</xml_diff>